<commit_message>
Fixed 2010 data for 3 cities
</commit_message>
<xml_diff>
--- a/Population/Manual_data_collection.xlsx
+++ b/Population/Manual_data_collection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://1sfu-my.sharepoint.com/personal/bsg13_sfu_ca/Documents/SFU Classes/CMPT 353/Final Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{9E305742-907F-47B8-87C1-4585D1BECFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B71D6EF4-02A2-4596-A83D-E95777B88B8F}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{9E305742-907F-47B8-87C1-4585D1BECFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5863D088-6110-4A56-AD20-95F0239A0927}"/>
   <bookViews>
-    <workbookView xWindow="8910" yWindow="3480" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3300" yWindow="3570" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="16">
   <si>
     <t>Fredericton</t>
   </si>
@@ -159,6 +159,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -424,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,7 +824,7 @@
       </c>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -832,7 +836,7 @@
       </c>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -844,7 +848,7 @@
       </c>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>8</v>
       </c>
@@ -856,7 +860,7 @@
       </c>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>8</v>
       </c>
@@ -868,7 +872,7 @@
       </c>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>9</v>
       </c>
@@ -880,7 +884,7 @@
       </c>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>9</v>
       </c>
@@ -892,7 +896,7 @@
       </c>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>9</v>
       </c>
@@ -904,7 +908,7 @@
       </c>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>9</v>
       </c>
@@ -916,7 +920,7 @@
       </c>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>10</v>
       </c>
@@ -928,7 +932,7 @@
       </c>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>10</v>
       </c>
@@ -940,75 +944,106 @@
       </c>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B43" s="6">
-        <v>2000</v>
+        <v>2020</v>
       </c>
       <c r="C43" s="4">
-        <v>227818</v>
+        <v>887642</v>
       </c>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B44" s="6">
+        <v>2000</v>
+      </c>
+      <c r="C44" s="4">
+        <v>227818</v>
+      </c>
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" s="6">
         <v>2010</v>
       </c>
-      <c r="C44" s="4">
+      <c r="C45" s="4">
         <v>229493</v>
       </c>
-      <c r="D44" s="2"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" s="6">
+        <v>2020</v>
+      </c>
+      <c r="C46" s="4">
+        <v>227470</v>
+      </c>
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B45" s="6">
+      <c r="B47" s="6">
         <v>2000</v>
       </c>
-      <c r="C45" s="4">
+      <c r="C47" s="4">
         <v>545524</v>
       </c>
-      <c r="D45" s="2"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="6">
+      <c r="B48" s="6">
         <v>2010</v>
       </c>
-      <c r="C46" s="4">
+      <c r="C48" s="4">
         <v>601222</v>
       </c>
-      <c r="D46" s="2"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
       <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C49" s="3">
+        <v>689447</v>
+      </c>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B41" r:id="rId1" tooltip="2000 United States census" display="https://en.wikipedia.org/wiki/2000_United_States_census" xr:uid="{726FFB01-812C-4587-945A-1CA1E13D1B91}"/>
     <hyperlink ref="B42" r:id="rId2" tooltip="2010 United States census" display="https://en.wikipedia.org/wiki/2010_United_States_census" xr:uid="{58A9EFE2-9CBF-4C2A-8954-483B1D1AC73D}"/>
-    <hyperlink ref="B43" r:id="rId3" tooltip="2000 United States census" display="https://en.wikipedia.org/wiki/2000_United_States_census" xr:uid="{66F5A81B-97F3-4D75-9026-4A1FB4102725}"/>
-    <hyperlink ref="B44" r:id="rId4" tooltip="2010 United States census" display="https://en.wikipedia.org/wiki/2010_United_States_census" xr:uid="{4A14FCC7-A1F9-4EB8-88C2-C55944F38DE4}"/>
-    <hyperlink ref="B45" r:id="rId5" tooltip="2000 United States census" display="https://en.wikipedia.org/wiki/2000_United_States_census" xr:uid="{C2A89F1B-7FAA-4B49-B8FF-88AC8208A169}"/>
-    <hyperlink ref="B46" r:id="rId6" tooltip="2010 United States census" display="https://en.wikipedia.org/wiki/2010_United_States_census" xr:uid="{55851167-37C1-4ADB-AF56-334317A402B8}"/>
+    <hyperlink ref="B44" r:id="rId3" tooltip="2000 United States census" display="https://en.wikipedia.org/wiki/2000_United_States_census" xr:uid="{66F5A81B-97F3-4D75-9026-4A1FB4102725}"/>
+    <hyperlink ref="B46" r:id="rId4" tooltip="2010 United States census" display="https://en.wikipedia.org/wiki/2010_United_States_census" xr:uid="{4A14FCC7-A1F9-4EB8-88C2-C55944F38DE4}"/>
+    <hyperlink ref="B47" r:id="rId5" tooltip="2000 United States census" display="https://en.wikipedia.org/wiki/2000_United_States_census" xr:uid="{C2A89F1B-7FAA-4B49-B8FF-88AC8208A169}"/>
+    <hyperlink ref="B48" r:id="rId6" tooltip="2010 United States census" display="https://en.wikipedia.org/wiki/2010_United_States_census" xr:uid="{55851167-37C1-4ADB-AF56-334317A402B8}"/>
+    <hyperlink ref="B45" r:id="rId7" tooltip="2010 United States census" display="https://en.wikipedia.org/wiki/2010_United_States_census" xr:uid="{4997F76E-1D6C-41EE-8665-D3DA09E26C2B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>